<commit_message>
added results to summary
</commit_message>
<xml_diff>
--- a/results/summary.xlsx
+++ b/results/summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fergusproctor/dev/hand_gesture_detection/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75F5637F-8DF9-A647-BADD-93997BB71466}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{705520C9-90FE-D04C-825C-7AC0B64E787E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="660" yWindow="580" windowWidth="28040" windowHeight="16940" activeTab="1" xr2:uid="{6889DBCB-A4B9-0347-AF58-7DB0AC317158}"/>
+    <workbookView xWindow="660" yWindow="580" windowWidth="28040" windowHeight="16940" activeTab="2" xr2:uid="{6889DBCB-A4B9-0347-AF58-7DB0AC317158}"/>
   </bookViews>
   <sheets>
     <sheet name="Training_Master" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="108">
   <si>
     <t>efficientnet_v2_s_data_2</t>
   </si>
@@ -359,6 +359,9 @@
   </si>
   <si>
     <t>Avg F1</t>
+  </si>
+  <si>
+    <t>efficientnet_v2_s_TL_only</t>
   </si>
 </sst>
 </file>
@@ -366,9 +369,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="178" formatCode="0.0%"/>
+    <numFmt numFmtId="164" formatCode="0.0%"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -391,6 +394,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -406,7 +415,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -451,19 +460,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -471,16 +491,16 @@
   </cellStyles>
   <dxfs count="5">
     <dxf>
-      <numFmt numFmtId="178" formatCode="0.0%"/>
+      <numFmt numFmtId="164" formatCode="0.0%"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="178" formatCode="0.0%"/>
+      <numFmt numFmtId="164" formatCode="0.0%"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="178" formatCode="0.0%"/>
+      <numFmt numFmtId="164" formatCode="0.0%"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="178" formatCode="0.0%"/>
+      <numFmt numFmtId="164" formatCode="0.0%"/>
     </dxf>
     <dxf>
       <font>
@@ -786,7 +806,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>mobilenet_asl_only</c:v>
+                  <c:v>efficientnet_v2_s_TL_only</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -822,34 +842,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>60.011494252873497</c:v>
+                  <c:v>40.979591836734599</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>74.896551724137893</c:v>
+                  <c:v>58.969387755101998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>79.931034482758605</c:v>
+                  <c:v>65.663265306122398</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>82.632183908045903</c:v>
+                  <c:v>69.102040816326493</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>84.655172413793096</c:v>
+                  <c:v>70.979591836734699</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>86.034482758620598</c:v>
+                  <c:v>72.806122448979593</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>87.057471264367805</c:v>
+                  <c:v>74.336734693877503</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>87.712643678160902</c:v>
+                  <c:v>75.244897959183604</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>88.425287356321803</c:v>
+                  <c:v>75.612244897959101</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>88.804597701149405</c:v>
+                  <c:v>76.520408163265301</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -870,7 +890,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>mobilenet_unified_dataset</c:v>
+                  <c:v>mobilenet_asl_only</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -906,34 +926,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>57.5</c:v>
+                  <c:v>60.011494252873497</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>68.683673469387699</c:v>
+                  <c:v>74.896551724137893</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>74.153061224489704</c:v>
+                  <c:v>79.931034482758605</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>76.0918367346938</c:v>
+                  <c:v>82.632183908045903</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>77.938775510203996</c:v>
+                  <c:v>84.655172413793096</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>79.724489795918302</c:v>
+                  <c:v>86.034482758620598</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>80.397959183673393</c:v>
+                  <c:v>87.057471264367805</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>81.040816326530603</c:v>
+                  <c:v>87.712643678160902</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>82.183673469387699</c:v>
+                  <c:v>88.425287356321803</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>82.2959183673469</c:v>
+                  <c:v>88.804597701149405</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -942,6 +962,90 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000003-894C-484A-A9B5-C127FE7761F0}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="4"/>
+          <c:order val="4"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Training_Master!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>mobilenet_unified_dataset</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent5"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent5"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Training_Master!$E$2:$E$11</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>57.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>68.683673469387699</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>74.153061224489704</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>76.0918367346938</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>77.938775510203996</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>79.724489795918302</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>80.397959183673393</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>81.040816326530603</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>82.183673469387699</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>82.2959183673469</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BF44-CD49-852F-98FDEFFD1BB1}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -1709,13 +1813,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
+      <xdr:col>4</xdr:col>
       <xdr:colOff>63500</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
+      <xdr:col>17</xdr:col>
       <xdr:colOff>762000</xdr:colOff>
       <xdr:row>32</xdr:row>
       <xdr:rowOff>101600</xdr:rowOff>
@@ -1747,11 +1851,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{701B96DA-5432-FB4E-B6FB-E51B40F31A7D}" name="Table1" displayName="Table1" ref="A1:D11" totalsRowShown="0">
-  <autoFilter ref="A1:D11" xr:uid="{701B96DA-5432-FB4E-B6FB-E51B40F31A7D}"/>
-  <tableColumns count="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{701B96DA-5432-FB4E-B6FB-E51B40F31A7D}" name="Table1" displayName="Table1" ref="A1:E11" totalsRowShown="0">
+  <autoFilter ref="A1:E11" xr:uid="{701B96DA-5432-FB4E-B6FB-E51B40F31A7D}"/>
+  <tableColumns count="5">
     <tableColumn id="2" xr3:uid="{EACAD312-CC20-CE42-A243-8B6DE827A9DC}" name="efficientnet_v2_s_data_2"/>
     <tableColumn id="3" xr3:uid="{A3951122-5458-DA4A-9F52-F99DBEA6BD6A}" name="efficientnet_v2_s_data3"/>
+    <tableColumn id="1" xr3:uid="{47936C53-7346-C444-B2C3-4DA57771CB3C}" name="efficientnet_v2_s_TL_only"/>
     <tableColumn id="4" xr3:uid="{D2F2BD24-EA36-3946-92CB-9AE21C99BA02}" name="mobilenet_asl_only"/>
     <tableColumn id="5" xr3:uid="{5A5DB86B-8A2D-D14F-8B48-B64224D90622}" name="mobilenet_unified_dataset"/>
   </tableColumns>
@@ -1760,8 +1865,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AC62320D-9655-EF4C-B8EA-36608277FB94}" name="Table2" displayName="Table2" ref="A1:E5" totalsRowShown="0">
-  <autoFilter ref="A1:E5" xr:uid="{AC62320D-9655-EF4C-B8EA-36608277FB94}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AC62320D-9655-EF4C-B8EA-36608277FB94}" name="Table2" displayName="Table2" ref="A1:E6" totalsRowShown="0">
+  <autoFilter ref="A1:E6" xr:uid="{AC62320D-9655-EF4C-B8EA-36608277FB94}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{FE794F7B-755D-0649-8A37-9594AA7BD3E2}" name="Network Instance" dataDxfId="4"/>
     <tableColumn id="2" xr3:uid="{72F9656E-87CB-F049-9738-BE0CA7473654}" name="Avg Accuracy" dataDxfId="3" dataCellStyle="Per cent"/>
@@ -2090,10 +2195,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8C95E17-8F27-5446-9B06-20F5D897935A}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:E20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2101,7 +2206,7 @@
     <col min="1" max="1" width="11.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2109,13 +2214,16 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>78.163265306122398</v>
       </c>
@@ -2123,13 +2231,16 @@
         <v>85.425287356321803</v>
       </c>
       <c r="C2">
+        <v>40.979591836734599</v>
+      </c>
+      <c r="D2">
         <v>60.011494252873497</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>57.5</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>83.132653061224403</v>
       </c>
@@ -2137,13 +2248,16 @@
         <v>88.885057471264304</v>
       </c>
       <c r="C3">
+        <v>58.969387755101998</v>
+      </c>
+      <c r="D3">
         <v>74.896551724137893</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>68.683673469387699</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>85.846938775510196</v>
       </c>
@@ -2151,13 +2265,16 @@
         <v>90.505747126436702</v>
       </c>
       <c r="C4">
+        <v>65.663265306122398</v>
+      </c>
+      <c r="D4">
         <v>79.931034482758605</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>74.153061224489704</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>86.897959183673393</v>
       </c>
@@ -2165,13 +2282,16 @@
         <v>91.367816091953998</v>
       </c>
       <c r="C5">
+        <v>69.102040816326493</v>
+      </c>
+      <c r="D5">
         <v>82.632183908045903</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>76.0918367346938</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>87.5</v>
       </c>
@@ -2179,13 +2299,16 @@
         <v>91.953999999999994</v>
       </c>
       <c r="C6">
+        <v>70.979591836734699</v>
+      </c>
+      <c r="D6">
         <v>84.655172413793096</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>77.938775510203996</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>92.765306122448905</v>
       </c>
@@ -2193,13 +2316,16 @@
         <v>96.988505747126396</v>
       </c>
       <c r="C7">
+        <v>72.806122448979593</v>
+      </c>
+      <c r="D7">
         <v>86.034482758620598</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>79.724489795918302</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>93.571428571428498</v>
       </c>
@@ -2207,13 +2333,16 @@
         <v>97.827586206896498</v>
       </c>
       <c r="C8">
+        <v>74.336734693877503</v>
+      </c>
+      <c r="D8">
         <v>87.057471264367805</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>80.397959183673393</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>94.489795918367307</v>
       </c>
@@ -2221,13 +2350,16 @@
         <v>98.091954022988503</v>
       </c>
       <c r="C9">
+        <v>75.244897959183604</v>
+      </c>
+      <c r="D9">
         <v>87.712643678160902</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>81.040816326530603</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>95.122448979591795</v>
       </c>
@@ -2235,13 +2367,16 @@
         <v>98.3333333333333</v>
       </c>
       <c r="C10">
+        <v>75.612244897959101</v>
+      </c>
+      <c r="D10">
         <v>88.425287356321803</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>82.183673469387699</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>95.785714285714207</v>
       </c>
@@ -2249,9 +2384,12 @@
         <v>98.816091954022994</v>
       </c>
       <c r="C11">
+        <v>76.520408163265301</v>
+      </c>
+      <c r="D11">
         <v>88.804597701149405</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>82.2959183673469</v>
       </c>
     </row>
@@ -2266,6 +2404,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
   <tableParts count="1">
@@ -2276,15 +2415,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1997F876-4A01-464A-8859-A7F43C9F3962}">
-  <dimension ref="A1:Y34"/>
+  <dimension ref="A1:AE34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="K19" sqref="K19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AB32" sqref="AB32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2297,8 +2436,11 @@
       <c r="U1" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="AA1" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>5</v>
       </c>
@@ -2347,8 +2489,20 @@
       <c r="Y2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="AB2" t="s">
+        <v>5</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>6</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>7</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -2409,8 +2563,23 @@
       <c r="Y3">
         <v>350</v>
       </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="AA3">
+        <v>0</v>
+      </c>
+      <c r="AB3">
+        <v>0.77955271565495199</v>
+      </c>
+      <c r="AC3">
+        <v>0.72403560830860503</v>
+      </c>
+      <c r="AD3">
+        <v>0.75076923076922997</v>
+      </c>
+      <c r="AE3">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>10</v>
       </c>
@@ -2471,8 +2640,23 @@
       <c r="Y4">
         <v>350</v>
       </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="AA4">
+        <v>1</v>
+      </c>
+      <c r="AB4">
+        <v>0.77386934673366803</v>
+      </c>
+      <c r="AC4">
+        <v>0.87749287749287697</v>
+      </c>
+      <c r="AD4">
+        <v>0.82242990654205606</v>
+      </c>
+      <c r="AE4">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -2533,8 +2717,23 @@
       <c r="Y5">
         <v>338</v>
       </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="AA5">
+        <v>2</v>
+      </c>
+      <c r="AB5">
+        <v>0.82172701949860705</v>
+      </c>
+      <c r="AC5">
+        <v>0.82172701949860705</v>
+      </c>
+      <c r="AD5">
+        <v>0.82172701949860705</v>
+      </c>
+      <c r="AE5">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>12</v>
       </c>
@@ -2595,8 +2794,23 @@
       <c r="Y6">
         <v>326</v>
       </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="AA6">
+        <v>3</v>
+      </c>
+      <c r="AB6">
+        <v>0.94426229508196702</v>
+      </c>
+      <c r="AC6">
+        <v>0.83478260869565202</v>
+      </c>
+      <c r="AD6">
+        <v>0.88615384615384596</v>
+      </c>
+      <c r="AE6">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -2657,8 +2871,23 @@
       <c r="Y7">
         <v>326</v>
       </c>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="AA7">
+        <v>4</v>
+      </c>
+      <c r="AB7">
+        <v>0.62711864406779605</v>
+      </c>
+      <c r="AC7">
+        <v>0.80185758513931804</v>
+      </c>
+      <c r="AD7">
+        <v>0.70380434782608603</v>
+      </c>
+      <c r="AE7">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -2719,8 +2948,23 @@
       <c r="Y8">
         <v>337</v>
       </c>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="AA8">
+        <v>5</v>
+      </c>
+      <c r="AB8">
+        <v>0.77237851662404</v>
+      </c>
+      <c r="AC8">
+        <v>0.87536231884057902</v>
+      </c>
+      <c r="AD8">
+        <v>0.82065217391304301</v>
+      </c>
+      <c r="AE8">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="9" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>15</v>
       </c>
@@ -2781,8 +3025,23 @@
       <c r="Y9">
         <v>344</v>
       </c>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="AA9">
+        <v>6</v>
+      </c>
+      <c r="AB9">
+        <v>0.80288461538461497</v>
+      </c>
+      <c r="AC9">
+        <v>0.84556962025316396</v>
+      </c>
+      <c r="AD9">
+        <v>0.82367447595561005</v>
+      </c>
+      <c r="AE9">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="10" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>16</v>
       </c>
@@ -2843,8 +3102,23 @@
       <c r="Y10">
         <v>331</v>
       </c>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="AA10">
+        <v>7</v>
+      </c>
+      <c r="AB10">
+        <v>0.86746987951807197</v>
+      </c>
+      <c r="AC10">
+        <v>0.82521489971346695</v>
+      </c>
+      <c r="AD10">
+        <v>0.84581497797356797</v>
+      </c>
+      <c r="AE10">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="11" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>17</v>
       </c>
@@ -2905,8 +3179,23 @@
       <c r="Y11">
         <v>321</v>
       </c>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="AA11">
+        <v>8</v>
+      </c>
+      <c r="AB11">
+        <v>0.75070028011204404</v>
+      </c>
+      <c r="AC11">
+        <v>0.81212121212121202</v>
+      </c>
+      <c r="AD11">
+        <v>0.78020378457059603</v>
+      </c>
+      <c r="AE11">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="12" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>18</v>
       </c>
@@ -2967,8 +3256,23 @@
       <c r="Y12">
         <v>322</v>
       </c>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="AA12">
+        <v>9</v>
+      </c>
+      <c r="AB12">
+        <v>0.74561403508771895</v>
+      </c>
+      <c r="AC12">
+        <v>0.75892857142857095</v>
+      </c>
+      <c r="AD12">
+        <v>0.75221238938053003</v>
+      </c>
+      <c r="AE12">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="13" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>19</v>
       </c>
@@ -3029,8 +3333,23 @@
       <c r="Y13">
         <v>342</v>
       </c>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="AA13">
+        <v>10</v>
+      </c>
+      <c r="AB13">
+        <v>0.790087463556851</v>
+      </c>
+      <c r="AC13">
+        <v>0.79941002949852502</v>
+      </c>
+      <c r="AD13">
+        <v>0.79472140762463295</v>
+      </c>
+      <c r="AE13">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -3091,8 +3410,23 @@
       <c r="Y14">
         <v>352</v>
       </c>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="AA14">
+        <v>11</v>
+      </c>
+      <c r="AB14">
+        <v>0.83113456464379898</v>
+      </c>
+      <c r="AC14">
+        <v>0.88235294117647001</v>
+      </c>
+      <c r="AD14">
+        <v>0.85597826086956497</v>
+      </c>
+      <c r="AE14">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>21</v>
       </c>
@@ -3153,8 +3487,23 @@
       <c r="Y15">
         <v>310</v>
       </c>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="AA15">
+        <v>12</v>
+      </c>
+      <c r="AB15">
+        <v>0.76996805111820998</v>
+      </c>
+      <c r="AC15">
+        <v>0.74153846153846104</v>
+      </c>
+      <c r="AD15">
+        <v>0.75548589341692696</v>
+      </c>
+      <c r="AE15">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>22</v>
       </c>
@@ -3215,8 +3564,23 @@
       <c r="Y16">
         <v>356</v>
       </c>
-    </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="AA16">
+        <v>13</v>
+      </c>
+      <c r="AB16">
+        <v>0.71502590673575095</v>
+      </c>
+      <c r="AC16">
+        <v>0.76666666666666605</v>
+      </c>
+      <c r="AD16">
+        <v>0.73994638069705099</v>
+      </c>
+      <c r="AE16">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="17" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>23</v>
       </c>
@@ -3277,8 +3641,23 @@
       <c r="Y17">
         <v>366</v>
       </c>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="AA17">
+        <v>14</v>
+      </c>
+      <c r="AB17">
+        <v>0.70161290322580605</v>
+      </c>
+      <c r="AC17">
+        <v>0.85855263157894701</v>
+      </c>
+      <c r="AD17">
+        <v>0.77218934911242598</v>
+      </c>
+      <c r="AE17">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="18" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>24</v>
       </c>
@@ -3339,8 +3718,23 @@
       <c r="Y18">
         <v>315</v>
       </c>
-    </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="AA18">
+        <v>15</v>
+      </c>
+      <c r="AB18">
+        <v>0.81114551083591302</v>
+      </c>
+      <c r="AC18">
+        <v>0.78678678678678604</v>
+      </c>
+      <c r="AD18">
+        <v>0.79878048780487798</v>
+      </c>
+      <c r="AE18">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="19" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>25</v>
       </c>
@@ -3401,8 +3795,23 @@
       <c r="Y19">
         <v>319</v>
       </c>
-    </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="AA19">
+        <v>16</v>
+      </c>
+      <c r="AB19">
+        <v>0.79754601226993804</v>
+      </c>
+      <c r="AC19">
+        <v>0.79754601226993804</v>
+      </c>
+      <c r="AD19">
+        <v>0.79754601226993804</v>
+      </c>
+      <c r="AE19">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="20" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>26</v>
       </c>
@@ -3463,8 +3872,23 @@
       <c r="Y20">
         <v>351</v>
       </c>
-    </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="AA20">
+        <v>17</v>
+      </c>
+      <c r="AB20">
+        <v>0.70550161812297696</v>
+      </c>
+      <c r="AC20">
+        <v>0.69648562300319405</v>
+      </c>
+      <c r="AD20">
+        <v>0.70096463022508004</v>
+      </c>
+      <c r="AE20">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="21" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>27</v>
       </c>
@@ -3525,8 +3949,23 @@
       <c r="Y21">
         <v>307</v>
       </c>
-    </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="AA21">
+        <v>18</v>
+      </c>
+      <c r="AB21">
+        <v>0.71713147410358502</v>
+      </c>
+      <c r="AC21">
+        <v>0.57692307692307598</v>
+      </c>
+      <c r="AD21">
+        <v>0.63943161634102996</v>
+      </c>
+      <c r="AE21">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="22" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>28</v>
       </c>
@@ -3587,8 +4026,23 @@
       <c r="Y22">
         <v>333</v>
       </c>
-    </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="AA22">
+        <v>19</v>
+      </c>
+      <c r="AB22">
+        <v>0.64431486880466404</v>
+      </c>
+      <c r="AC22">
+        <v>0.64057971014492698</v>
+      </c>
+      <c r="AD22">
+        <v>0.64244186046511598</v>
+      </c>
+      <c r="AE22">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="23" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>29</v>
       </c>
@@ -3649,8 +4103,23 @@
       <c r="Y23">
         <v>365</v>
       </c>
-    </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="AA23">
+        <v>20</v>
+      </c>
+      <c r="AB23">
+        <v>0.64516129032257996</v>
+      </c>
+      <c r="AC23">
+        <v>0.52785923753665598</v>
+      </c>
+      <c r="AD23">
+        <v>0.58064516129032195</v>
+      </c>
+      <c r="AE23">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="24" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>30</v>
       </c>
@@ -3711,8 +4180,23 @@
       <c r="Y24">
         <v>320</v>
       </c>
-    </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="AA24">
+        <v>21</v>
+      </c>
+      <c r="AB24">
+        <v>0.83396226415094299</v>
+      </c>
+      <c r="AC24">
+        <v>0.62784090909090895</v>
+      </c>
+      <c r="AD24">
+        <v>0.716369529983792</v>
+      </c>
+      <c r="AE24">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="25" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>31</v>
       </c>
@@ -3773,8 +4257,23 @@
       <c r="Y25">
         <v>309</v>
       </c>
-    </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="AA25">
+        <v>22</v>
+      </c>
+      <c r="AB25">
+        <v>0.91603053435114501</v>
+      </c>
+      <c r="AC25">
+        <v>0.69565217391304301</v>
+      </c>
+      <c r="AD25">
+        <v>0.79077429983525505</v>
+      </c>
+      <c r="AE25">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="26" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>32</v>
       </c>
@@ -3835,8 +4334,23 @@
       <c r="Y26">
         <v>346</v>
       </c>
-    </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="AA26">
+        <v>23</v>
+      </c>
+      <c r="AB26">
+        <v>0.69817073170731703</v>
+      </c>
+      <c r="AC26">
+        <v>0.671554252199413</v>
+      </c>
+      <c r="AD26">
+        <v>0.68460388639760805</v>
+      </c>
+      <c r="AE26">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="27" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>33</v>
       </c>
@@ -3897,8 +4411,23 @@
       <c r="Y27">
         <v>334</v>
       </c>
-    </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="AA27">
+        <v>24</v>
+      </c>
+      <c r="AB27">
+        <v>0.80308880308880304</v>
+      </c>
+      <c r="AC27">
+        <v>0.62650602409638501</v>
+      </c>
+      <c r="AD27">
+        <v>0.70389170896785103</v>
+      </c>
+      <c r="AE27">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="28" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>34</v>
       </c>
@@ -3959,8 +4488,23 @@
       <c r="Y28">
         <v>343</v>
       </c>
-    </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="AA28">
+        <v>25</v>
+      </c>
+      <c r="AB28">
+        <v>0.67919799498746802</v>
+      </c>
+      <c r="AC28">
+        <v>0.77207977207977196</v>
+      </c>
+      <c r="AD28">
+        <v>0.72266666666666601</v>
+      </c>
+      <c r="AE28">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="29" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>35</v>
       </c>
@@ -4021,8 +4565,23 @@
       <c r="Y29">
         <v>364</v>
       </c>
-    </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="AA29">
+        <v>26</v>
+      </c>
+      <c r="AB29">
+        <v>0.76630434782608603</v>
+      </c>
+      <c r="AC29">
+        <v>0.90675241157556197</v>
+      </c>
+      <c r="AD29">
+        <v>0.83063328424153104</v>
+      </c>
+      <c r="AE29">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="30" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>36</v>
       </c>
@@ -4083,8 +4642,23 @@
       <c r="Y30">
         <v>342</v>
       </c>
-    </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="AA30">
+        <v>27</v>
+      </c>
+      <c r="AB30">
+        <v>0.99380804953560298</v>
+      </c>
+      <c r="AC30">
+        <v>0.95535714285714202</v>
+      </c>
+      <c r="AD30">
+        <v>0.97420333839150197</v>
+      </c>
+      <c r="AE30">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="31" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>37</v>
       </c>
@@ -4145,8 +4719,23 @@
       <c r="Y31">
         <v>381</v>
       </c>
-    </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="AA31">
+        <v>28</v>
+      </c>
+      <c r="AB31">
+        <v>0.79190751445086704</v>
+      </c>
+      <c r="AC31">
+        <v>0.89250814332247497</v>
+      </c>
+      <c r="AD31">
+        <v>0.83920367534456297</v>
+      </c>
+      <c r="AE31">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="32" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>38</v>
       </c>
@@ -4207,8 +4796,23 @@
       <c r="Y32">
         <v>0.83132653061224404</v>
       </c>
-    </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="AA32" t="s">
+        <v>38</v>
+      </c>
+      <c r="AB32">
+        <v>0.77265306122448896</v>
+      </c>
+      <c r="AC32">
+        <v>0.77265306122448896</v>
+      </c>
+      <c r="AD32">
+        <v>0.77265306122448896</v>
+      </c>
+      <c r="AE32">
+        <v>0.77265306122448896</v>
+      </c>
+    </row>
+    <row r="33" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>39</v>
       </c>
@@ -4269,8 +4873,23 @@
       <c r="Y33">
         <v>9800</v>
       </c>
-    </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.2">
+      <c r="AA33" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB33">
+        <v>0.77574749143454402</v>
+      </c>
+      <c r="AC33">
+        <v>0.77241532164656601</v>
+      </c>
+      <c r="AD33">
+        <v>0.77061791732858298</v>
+      </c>
+      <c r="AE33">
+        <v>9800</v>
+      </c>
+    </row>
+    <row r="34" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>40</v>
       </c>
@@ -4329,6 +4948,21 @@
         <v>0.831624565831106</v>
       </c>
       <c r="Y34">
+        <v>9800</v>
+      </c>
+      <c r="AA34" t="s">
+        <v>40</v>
+      </c>
+      <c r="AB34">
+        <v>0.77681468441357704</v>
+      </c>
+      <c r="AC34">
+        <v>0.77265306122448896</v>
+      </c>
+      <c r="AD34">
+        <v>0.77131401602783101</v>
+      </c>
+      <c r="AE34">
         <v>9800</v>
       </c>
     </row>
@@ -4339,10 +4973,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{760D6559-A44D-5340-86A0-E44949F51765}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4439,6 +5073,23 @@
         <v>0.83232205187749397</v>
       </c>
     </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="B6" s="8">
+        <v>0.77265306122448896</v>
+      </c>
+      <c r="C6" s="8">
+        <v>0.77574749143454402</v>
+      </c>
+      <c r="D6" s="8">
+        <v>0.77241532164656601</v>
+      </c>
+      <c r="E6" s="8">
+        <v>0.77061791732858298</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>